<commit_message>
Added New Error Codes
</commit_message>
<xml_diff>
--- a/APIs List.xlsx
+++ b/APIs List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amrkh\Desktop\YelloCo\5.Fifth Task\AMS-DBFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A3CB95-BE12-44C9-A1ED-903C9A00EA56}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6A9676-DEBD-41C3-AC34-969D0BFDB158}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D06956B6-4667-4710-953E-65E9902BA318}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2766" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="605">
   <si>
     <t>Serial Number</t>
   </si>
@@ -1829,12 +1829,6 @@
     <t>incident/getCategoriesByDepID</t>
   </si>
   <si>
-    <t>A01004020001</t>
-  </si>
-  <si>
-    <t>A01004020002</t>
-  </si>
-  <si>
     <t>No Response Sequence Number Provided</t>
   </si>
   <si>
@@ -1845,6 +1839,12 @@
   </si>
   <si>
     <t>Assigns a Vehicle to a response</t>
+  </si>
+  <si>
+    <t>A01004011001</t>
+  </si>
+  <si>
+    <t>A01004011002</t>
   </si>
 </sst>
 </file>
@@ -1975,17 +1975,17 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2304,7 +2304,7 @@
   <dimension ref="A1:J287"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A191" zoomScale="124" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A202" sqref="A202"/>
+      <selection activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7395,16 +7395,16 @@
     </row>
     <row r="200" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B200" s="3">
         <v>153</v>
       </c>
-      <c r="C200" s="13" t="s">
+      <c r="C200" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="D200" s="3" t="s">
         <v>601</v>
-      </c>
-      <c r="D200" s="3" t="s">
-        <v>603</v>
       </c>
       <c r="E200" s="3" t="s">
         <v>178</v>
@@ -7412,30 +7412,30 @@
       <c r="F200" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="G200" s="14"/>
+      <c r="G200" s="12"/>
       <c r="H200" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="I200" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="J200" s="14"/>
+        <v>602</v>
+      </c>
+      <c r="I200" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J200" s="12"/>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B201" s="3"/>
+      <c r="C201" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="B201" s="3"/>
-      <c r="C201" s="14" t="s">
-        <v>602</v>
-      </c>
       <c r="D201" s="3"/>
-      <c r="E201" s="14"/>
-      <c r="F201" s="14"/>
-      <c r="G201" s="14"/>
-      <c r="H201" s="14"/>
-      <c r="I201" s="14"/>
-      <c r="J201" s="14"/>
+      <c r="E201" s="12"/>
+      <c r="F201" s="12"/>
+      <c r="G201" s="12"/>
+      <c r="H201" s="12"/>
+      <c r="I201" s="12"/>
+      <c r="J201" s="12"/>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B202" s="1"/>
@@ -7475,10 +7475,10 @@
       <c r="D210" s="1"/>
     </row>
     <row r="211" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B211" s="11" t="s">
+      <c r="B211" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="C211" s="11"/>
+      <c r="C211" s="13"/>
       <c r="D211" s="1"/>
     </row>
     <row r="212" spans="2:4" x14ac:dyDescent="0.3">
@@ -7554,10 +7554,10 @@
       <c r="D220" s="1"/>
     </row>
     <row r="221" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B221" s="12" t="s">
+      <c r="B221" s="14" t="s">
         <v>582</v>
       </c>
-      <c r="C221" s="12"/>
+      <c r="C221" s="14"/>
       <c r="D221" s="1"/>
     </row>
     <row r="222" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>